<commit_message>
Fix optimization, build geom model
</commit_message>
<xml_diff>
--- a/station_in_config/Axis.xlsx
+++ b/station_in_config/Axis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="1680" windowWidth="21735" windowHeight="8385"/>
+    <workbookView xWindow="8790" yWindow="195" windowWidth="9120" windowHeight="4155"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,7 +404,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Coord evaluation implemented + data format Cs, Point
</commit_message>
<xml_diff>
--- a/station_in_config/Axis.xlsx
+++ b/station_in_config/Axis.xlsx
@@ -65,6 +65,8 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -404,7 +406,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>